<commit_message>
Added specification of c_vars, p_vars, g_vars
</commit_message>
<xml_diff>
--- a/lasi/G2A LASI Family Variable List.xlsx
+++ b/lasi/G2A LASI Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3205AD3-9FD4-4981-8262-6ED497C92682}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B24F6F-6105-4FB9-86AC-73D634EA6A5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="329">
   <si>
     <t>state</t>
   </si>
@@ -996,6 +996,18 @@
   </si>
   <si>
     <t>hh_consumption</t>
+  </si>
+  <si>
+    <t>Length of current marriage</t>
+  </si>
+  <si>
+    <t>r1mcurln</t>
+  </si>
+  <si>
+    <t>s1mcurln</t>
+  </si>
+  <si>
+    <t>lengthmar</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1063,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1432,7 +1464,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H65" sqref="H65:H68"/>
+      <selection pane="bottomLeft" activeCell="B70" sqref="A70:XFD70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1931,68 +1963,65 @@
         <v>269</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="5" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A24" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="G24" t="s">
+        <v>326</v>
+      </c>
+      <c r="H24" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="H24" s="6" t="s">
+      <c r="H25" s="6" t="s">
         <v>207</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="D25" s="5"/>
-      <c r="G25" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>315</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>122</v>
-      </c>
+    <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D26" s="5"/>
       <c r="G26" s="6" t="s">
-        <v>209</v>
+        <v>314</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>210</v>
+        <v>315</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
@@ -2000,19 +2029,19 @@
         <v>98</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
@@ -2020,22 +2049,19 @@
         <v>98</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="J28" t="s">
-        <v>164</v>
+        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
@@ -2043,22 +2069,22 @@
         <v>98</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>84</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J29" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
@@ -2066,19 +2092,22 @@
         <v>98</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>220</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>217</v>
+        <v>78</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="J30" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
@@ -2086,16 +2115,19 @@
         <v>98</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
+      </c>
+      <c r="J31" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
@@ -2103,19 +2135,16 @@
         <v>98</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>12</v>
+        <v>219</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D32" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
@@ -2123,22 +2152,19 @@
         <v>98</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>111</v>
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>130</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="J33" t="s">
-        <v>208</v>
+        <v>226</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
@@ -2146,19 +2172,22 @@
         <v>98</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>82</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" t="s">
-        <v>175</v>
-      </c>
-      <c r="H34" t="s">
-        <v>176</v>
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="J34" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
@@ -2166,19 +2195,19 @@
         <v>98</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H35" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
@@ -2186,19 +2215,19 @@
         <v>98</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G36" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H36" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
@@ -2206,19 +2235,19 @@
         <v>98</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G37" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H37" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
@@ -2226,19 +2255,19 @@
         <v>98</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="G38" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
@@ -2246,19 +2275,19 @@
         <v>98</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H39" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
@@ -2266,24 +2295,19 @@
         <v>98</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>133</v>
+        <v>52</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>135</v>
+        <v>58</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="I40" s="3"/>
-      <c r="J40" t="s">
-        <v>142</v>
+        <v>171</v>
+      </c>
+      <c r="G40" t="s">
+        <v>184</v>
+      </c>
+      <c r="H40" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
@@ -2291,24 +2315,24 @@
         <v>98</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F41" s="3"/>
       <c r="G41" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="I41" s="3"/>
       <c r="J41" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
@@ -2316,51 +2340,53 @@
         <v>98</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="I42" s="3"/>
+      <c r="J42" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>26</v>
+        <v>139</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>98</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D44" t="s">
-        <v>94</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="J44" t="s">
-        <v>208</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
@@ -2368,19 +2394,19 @@
         <v>98</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J45" t="s">
         <v>208</v>
@@ -2391,13 +2417,22 @@
         <v>98</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="D46" t="s">
-        <v>103</v>
+        <v>97</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="J46" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
@@ -2405,13 +2440,13 @@
         <v>98</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
@@ -2419,21 +2454,24 @@
         <v>98</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>62</v>
+        <v>108</v>
+      </c>
+      <c r="D48" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B49" t="s">
-        <v>4</v>
+      <c r="B49" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
@@ -2441,21 +2479,21 @@
         <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>30</v>
+      <c r="B51" t="s">
+        <v>5</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
@@ -2463,22 +2501,10 @@
         <v>98</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D52" t="s">
-        <v>95</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J52" t="s">
-        <v>208</v>
+        <v>63</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
@@ -2486,19 +2512,19 @@
         <v>98</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D53" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="J53" t="s">
         <v>208</v>
@@ -2509,13 +2535,22 @@
         <v>98</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>105</v>
+        <v>96</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="J54" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
@@ -2523,13 +2558,13 @@
         <v>98</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
@@ -2537,10 +2572,13 @@
         <v>98</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>33</v>
+        <v>102</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>85</v>
+        <v>110</v>
+      </c>
+      <c r="D56" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
@@ -2548,22 +2586,10 @@
         <v>98</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E57" t="s">
-        <v>145</v>
-      </c>
-      <c r="G57" t="s">
-        <v>239</v>
-      </c>
-      <c r="H57" t="s">
-        <v>240</v>
-      </c>
-      <c r="J57" t="s">
-        <v>147</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
@@ -2571,19 +2597,19 @@
         <v>98</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E58" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G58" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="H58" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="J58" t="s">
         <v>147</v>
@@ -2594,16 +2620,22 @@
         <v>98</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>144</v>
       </c>
       <c r="G59" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H59" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="J59" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
@@ -2611,19 +2643,16 @@
         <v>98</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E60" t="s">
-        <v>148</v>
+        <v>88</v>
       </c>
       <c r="G60" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="H60" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
@@ -2631,19 +2660,19 @@
         <v>98</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G61" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="H61" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
@@ -2651,42 +2680,39 @@
         <v>98</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>150</v>
+        <v>14</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>151</v>
+        <v>67</v>
       </c>
       <c r="E62" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="G62" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="H62" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>42</v>
+        <v>150</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="D63" t="s">
-        <v>114</v>
+        <v>151</v>
+      </c>
+      <c r="E63" t="s">
+        <v>152</v>
       </c>
       <c r="G63" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H63" t="s">
-        <v>250</v>
-      </c>
-      <c r="J63" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
@@ -2694,120 +2720,140 @@
         <v>74</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D64" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G64" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H64" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J64" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="D65" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G65" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="H65" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+      <c r="J65" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>259</v>
+        <v>44</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
+      </c>
+      <c r="D66" t="s">
+        <v>116</v>
       </c>
       <c r="G66" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="H66" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="G67" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H67" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="G68" t="s">
+        <v>263</v>
+      </c>
+      <c r="H68" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B69" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="C69" s="3" t="s">
         <v>316</v>
       </c>
-      <c r="G68" t="s">
+      <c r="G69" t="s">
         <v>265</v>
       </c>
-      <c r="H68" t="s">
+      <c r="H69" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B69"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B70"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B71"/>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B72"/>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B73"/>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B74"/>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B75"/>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B76"/>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B77"/>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.35">
@@ -2820,32 +2866,41 @@
       <c r="D86" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D87:D1048576 D3:D33 D1 E34:E39 D43:D50 E40:I42 D52:D85 E60:I62 E18:J18 G44:H45 E57:I58 G63:H64 G65:G68">
-    <cfRule type="duplicateValues" dxfId="9" priority="11"/>
+  <conditionalFormatting sqref="D87:D1048576 D3:D23 D1 E35:E40 D44:D51 E41:I43 D53:D85 E61:I63 E18:J18 G45:H46 E58:I59 G64:H65 G66:G69 D25:D34">
+    <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D86">
-    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:B1048576 B1:B15 B78:B89 B17:B68">
-    <cfRule type="duplicateValues" dxfId="7" priority="9"/>
+  <conditionalFormatting sqref="B94:B1048576 B1:B15 B78:B89 B17:B23 B25:B69">
+    <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E7">
-    <cfRule type="duplicateValues" dxfId="5" priority="27"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="30"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5 F3:I7">
-    <cfRule type="duplicateValues" dxfId="4" priority="29"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G52:H53">
+  <conditionalFormatting sqref="G53:H54">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:E16">
+    <cfRule type="duplicateValues" dxfId="4" priority="51"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D24 G24">
     <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E12:E16">
-    <cfRule type="duplicateValues" dxfId="2" priority="48"/>
+  <conditionalFormatting sqref="B24">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H65:H68">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="H24">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66:H69">
+    <cfRule type="duplicateValues" dxfId="0" priority="70"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated LASI code for concordance with final set of variables
</commit_message>
<xml_diff>
--- a/lasi/G2A LASI Family Variable List.xlsx
+++ b/lasi/G2A LASI Family Variable List.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B24F6F-6105-4FB9-86AC-73D634EA6A5D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F396DA15-A073-49A3-BE41-D427E9712AD8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="335">
   <si>
     <t>state</t>
   </si>
@@ -146,9 +146,6 @@
     <t>Smoking current</t>
   </si>
   <si>
-    <t>Alcohol</t>
-  </si>
-  <si>
     <t>Caste of head of household</t>
   </si>
   <si>
@@ -1008,6 +1005,27 @@
   </si>
   <si>
     <t>lengthmar</t>
+  </si>
+  <si>
+    <t>Binge drinking</t>
+  </si>
+  <si>
+    <t>Any alcohol in last 3 months</t>
+  </si>
+  <si>
+    <t>r1drinkb</t>
+  </si>
+  <si>
+    <t>s1drinkb</t>
+  </si>
+  <si>
+    <t>heavydrinker</t>
+  </si>
+  <si>
+    <t>raedyrs</t>
+  </si>
+  <si>
+    <t>s1edyrs</t>
   </si>
 </sst>
 </file>
@@ -1460,11 +1478,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271C18A0-0761-4BF3-9F1D-A36E2FCBDA0F}">
-  <dimension ref="A1:J86"/>
+  <dimension ref="A1:J87"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B70" sqref="A70:XFD70"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1482,34 +1500,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1534,13 +1552,13 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1554,19 +1572,19 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1589,13 +1607,13 @@
         <v>9</v>
       </c>
       <c r="G5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H5" t="s">
+        <v>269</v>
+      </c>
+      <c r="J5" t="s">
         <v>270</v>
-      </c>
-      <c r="H5" t="s">
-        <v>270</v>
-      </c>
-      <c r="J5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1609,16 +1627,16 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" t="s">
+        <v>201</v>
+      </c>
+      <c r="H6" t="s">
         <v>202</v>
-      </c>
-      <c r="H6" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1626,16 +1644,16 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="G7" t="s">
         <v>319</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="G7" t="s">
-        <v>320</v>
-      </c>
       <c r="H7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -1646,7 +1664,7 @@
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D8" s="3"/>
     </row>
@@ -1658,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -1670,13 +1688,13 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>25</v>
@@ -1687,10 +1705,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>10</v>
@@ -1714,97 +1732,97 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>73</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>162</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>36</v>
@@ -1813,73 +1831,73 @@
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
+        <v>199</v>
+      </c>
+      <c r="H17" t="s">
         <v>200</v>
-      </c>
-      <c r="H17" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H18" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="I18" s="3"/>
       <c r="J18" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>192</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G19" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>37</v>
@@ -1890,906 +1908,911 @@
       <c r="D20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>194</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+        <v>156</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>334</v>
+      </c>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="D22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>257</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>258</v>
       </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>158</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="D23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H23" s="3" t="s">
         <v>267</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>268</v>
       </c>
       <c r="I23" s="3"/>
       <c r="J23" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="G24" t="s">
         <v>325</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>326</v>
-      </c>
-      <c r="H24" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="H25" s="6" t="s">
+      <c r="J25" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>312</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>313</v>
       </c>
       <c r="D26" s="5"/>
       <c r="G26" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>314</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>315</v>
-      </c>
       <c r="J26" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G27" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G28" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H28" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="H28" s="6" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G29" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="H29" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H29" s="6" t="s">
-        <v>214</v>
-      </c>
       <c r="J29" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>329</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="J30" t="s">
         <v>125</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="J30" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>220</v>
+        <v>328</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>217</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="D31" s="3"/>
       <c r="G31" s="6" t="s">
-        <v>221</v>
+        <v>330</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="J31" t="s">
-        <v>129</v>
+        <v>331</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>219</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>224</v>
+        <v>221</v>
+      </c>
+      <c r="J32" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>12</v>
+        <v>218</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s">
-        <v>130</v>
+        <v>217</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>111</v>
+        <v>90</v>
+      </c>
+      <c r="D34" t="s">
+        <v>129</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="J34" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G35" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" t="s">
-        <v>176</v>
+        <v>82</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="J35" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G36" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="H36" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G37" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="H37" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G38" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="H38" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G39" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="H39" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G40" t="s">
+        <v>182</v>
+      </c>
+      <c r="H40" t="s">
         <v>184</v>
-      </c>
-      <c r="H40" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>135</v>
+        <v>57</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="I41" s="3"/>
-      <c r="J41" t="s">
-        <v>142</v>
+        <v>170</v>
+      </c>
+      <c r="G41" t="s">
+        <v>183</v>
+      </c>
+      <c r="H41" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="E42" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>138</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I42" s="3"/>
       <c r="J42" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>189</v>
+      </c>
       <c r="I43" s="3"/>
+      <c r="J43" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" t="s">
-        <v>94</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="J45" t="s">
-        <v>208</v>
+        <v>58</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D46" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="J46" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>99</v>
+        <v>28</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="J47" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>100</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>62</v>
+        <v>107</v>
+      </c>
+      <c r="D49" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B50" t="s">
-        <v>4</v>
+        <v>97</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>30</v>
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>5</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" t="s">
-        <v>95</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="J53" t="s">
-        <v>208</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D54" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J54" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>105</v>
+        <v>95</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="J55" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D56" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>33</v>
+        <v>101</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>85</v>
+        <v>109</v>
+      </c>
+      <c r="D57" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" t="s">
-        <v>145</v>
-      </c>
-      <c r="G58" t="s">
-        <v>239</v>
-      </c>
-      <c r="H58" t="s">
-        <v>240</v>
-      </c>
-      <c r="J58" t="s">
-        <v>147</v>
+        <v>84</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E59" t="s">
         <v>144</v>
       </c>
       <c r="G59" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H59" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="E60" t="s">
+        <v>143</v>
       </c>
       <c r="G60" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="H60" t="s">
-        <v>242</v>
+        <v>237</v>
+      </c>
+      <c r="J60" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E61" t="s">
-        <v>148</v>
+        <v>87</v>
       </c>
       <c r="G61" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="H61" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E62" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H62" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>150</v>
+        <v>14</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>151</v>
+        <v>66</v>
       </c>
       <c r="E63" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="G63" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H63" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="D64" t="s">
-        <v>114</v>
+        <v>150</v>
+      </c>
+      <c r="E64" t="s">
+        <v>151</v>
       </c>
       <c r="G64" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H64" t="s">
-        <v>250</v>
-      </c>
-      <c r="J64" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D65" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G65" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="H65" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="J65" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="D66" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G66" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="H66" t="s">
-        <v>261</v>
+        <v>252</v>
+      </c>
+      <c r="J66" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>259</v>
+        <v>43</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
+      </c>
+      <c r="D67" t="s">
+        <v>115</v>
       </c>
       <c r="G67" t="s">
         <v>260</v>
@@ -2800,40 +2823,54 @@
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="G68" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="H68" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="G69" t="s">
+        <v>262</v>
+      </c>
+      <c r="H69" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A70" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="G70" t="s">
         <v>264</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="G69" t="s">
-        <v>265</v>
-      </c>
-      <c r="H69" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B70"/>
+      <c r="H70" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B71"/>
@@ -2856,23 +2893,26 @@
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B77"/>
     </row>
-    <row r="81" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D81" s="3"/>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="B78"/>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" s="3"/>
     </row>
-    <row r="86" spans="4:4" x14ac:dyDescent="0.35">
-      <c r="D86" s="3"/>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D87" s="3"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D87:D1048576 D3:D23 D1 E35:E40 D44:D51 E41:I43 D53:D85 E61:I63 E18:J18 G45:H46 E58:I59 G64:H65 G66:G69 D25:D34">
+  <conditionalFormatting sqref="D88:D1048576 D3:D23 D1 E36:E41 D45:D52 E42:I44 D54:D86 E62:I64 E18:J18 G46:H47 E59:I60 G65:H66 G67:G70 D25:D35">
     <cfRule type="duplicateValues" dxfId="11" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D86">
+  <conditionalFormatting sqref="D87">
     <cfRule type="duplicateValues" dxfId="10" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B94:B1048576 B1:B15 B78:B89 B17:B23 B25:B69">
+  <conditionalFormatting sqref="B95:B1048576 B1:B15 B79:B90 B17:B23 B25:B70">
     <cfRule type="duplicateValues" dxfId="9" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
@@ -2884,7 +2924,7 @@
   <conditionalFormatting sqref="J5 F3:I7">
     <cfRule type="duplicateValues" dxfId="6" priority="32"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G53:H54">
+  <conditionalFormatting sqref="G54:H55">
     <cfRule type="duplicateValues" dxfId="5" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E16">
@@ -2899,7 +2939,7 @@
   <conditionalFormatting sqref="H24">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H66:H69">
+  <conditionalFormatting sqref="H67:H70">
     <cfRule type="duplicateValues" dxfId="0" priority="70"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2922,10 +2962,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" t="s">
         <v>272</v>
-      </c>
-      <c r="B1" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2933,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -2941,7 +2981,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2949,7 +2989,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -2957,7 +2997,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
@@ -2965,7 +3005,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2973,7 +3013,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
@@ -2981,7 +3021,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
@@ -2989,7 +3029,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -2997,7 +3037,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3005,7 +3045,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3013,7 +3053,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
@@ -3021,7 +3061,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
@@ -3029,7 +3069,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
@@ -3037,7 +3077,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
@@ -3045,7 +3085,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
@@ -3053,7 +3093,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
@@ -3061,7 +3101,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
@@ -3069,7 +3109,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
@@ -3077,7 +3117,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
@@ -3085,7 +3125,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
@@ -3093,7 +3133,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
@@ -3101,7 +3141,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
@@ -3109,7 +3149,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
@@ -3117,7 +3157,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
@@ -3125,7 +3165,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
@@ -3133,7 +3173,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
@@ -3141,7 +3181,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
@@ -3149,7 +3189,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
@@ -3157,7 +3197,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
@@ -3165,7 +3205,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
@@ -3173,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
@@ -3181,7 +3221,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
@@ -3189,7 +3229,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
@@ -3197,7 +3237,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
@@ -3205,7 +3245,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit after response to reviewer comments, and calculating exact 95% CI
</commit_message>
<xml_diff>
--- a/lasi/G2A LASI Family Variable List.xlsx
+++ b/lasi/G2A LASI Family Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C19ACD5-8C57-405D-9512-5ED8128C142D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84904FA7-82B3-4FB3-B269-7462CC5001B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="11010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wave1" sheetId="6" r:id="rId1"/>
@@ -1480,7 +1480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271C18A0-0761-4BF3-9F1D-A36E2FCBDA0F}">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
     </sheetView>
@@ -2951,8 +2951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516FB498-DDE8-483E-BF1C-FF0717D5B9F0}">
   <dimension ref="A1:B36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>